<commit_message>
lisasin III juhtrühma slaidid, täpsustasin kulumudelit
</commit_message>
<xml_diff>
--- a/Kulumudel/ITAO teenuse kulumudel.xlsx
+++ b/Kulumudel/ITAO teenuse kulumudel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mts.local\dfs$\profiilid\risto.hinno\My Documents\Töö\Teenuse kulu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\GitHub\riigiteenused\Kulumudel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Risto Hinno</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Risto Hinno:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+SAPist välja järgnevad read: Admin. kulud (bürootarbed, side-, postikulud jm), Lähetuskulud, Koolituskulud, Kinnistute, hoonete, ruumide maj.kulud, IKT kulud (sh seadmete rent), Inventar, Töötervishoiu kulud ning jagada summa inimeste arvuga. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
@@ -110,7 +144,7 @@
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +199,19 @@
       <family val="2"/>
       <charset val="186"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -723,11 +770,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1204,5 +1251,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>